<commit_message>
Mô tả các chức năng cần hiện thực
Cập nhật trong sheet4 file excel
</commit_message>
<xml_diff>
--- a/N65_HappyLunch.xlsx
+++ b/N65_HappyLunch.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\apk\git\Happy_Lunch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52902F87-84FF-4988-AA3D-1F65AAAFA755}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDEA9927-9736-46E8-857F-EE7182294C3F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15996" windowHeight="8376" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15996" windowHeight="8376" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="194">
   <si>
     <t>NHÓM 65: HAPPY LUNCH</t>
   </si>
@@ -458,6 +459,153 @@
   </si>
   <si>
     <t>Sửa một số bug đang tồn tại</t>
+  </si>
+  <si>
+    <t>Chức năng</t>
+  </si>
+  <si>
+    <t>Người thực hiện</t>
+  </si>
+  <si>
+    <t>Tình trạng</t>
+  </si>
+  <si>
+    <t>Chưa hiện thực</t>
+  </si>
+  <si>
+    <t>Loại</t>
+  </si>
+  <si>
+    <t>Giao diện</t>
+  </si>
+  <si>
+    <t>Customer</t>
+  </si>
+  <si>
+    <t>Home</t>
+  </si>
+  <si>
+    <t>Tìm kiếm</t>
+  </si>
+  <si>
+    <t>Thông báo(chuông)</t>
+  </si>
+  <si>
+    <t>Mô tả</t>
+  </si>
+  <si>
+    <t>Chọn món ăn</t>
+  </si>
+  <si>
+    <t>Second shop</t>
+  </si>
+  <si>
+    <t>Shopping</t>
+  </si>
+  <si>
+    <t>Trả món ăn</t>
+  </si>
+  <si>
+    <t>Cập nhật thời gian</t>
+  </si>
+  <si>
+    <t>Hiện thị đúng thời gian đã hẹn lấy món ăn</t>
+  </si>
+  <si>
+    <t>Lấy thời gian mà người dùng đầu tiên đặt món hẹn lấy</t>
+  </si>
+  <si>
+    <t>Chọn số lượng muốn trả món ăn</t>
+  </si>
+  <si>
+    <t>Account</t>
+  </si>
+  <si>
+    <t>Kiểm tra tài khoản</t>
+  </si>
+  <si>
+    <t>In ra số coin hiện có</t>
+  </si>
+  <si>
+    <t>Cài đặt tài khoản</t>
+  </si>
+  <si>
+    <t>Đổi thông tin</t>
+  </si>
+  <si>
+    <t>Kiểm tra hóa đơn</t>
+  </si>
+  <si>
+    <t>Git</t>
+  </si>
+  <si>
+    <t>Chưa đồng bộ</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Quên mật khẩu</t>
+  </si>
+  <si>
+    <t>Employee</t>
+  </si>
+  <si>
+    <t>Ordered</t>
+  </si>
+  <si>
+    <t>Cập nhật status</t>
+  </si>
+  <si>
+    <t>Hiện dấu tích (V) nếu đã nhận món ăn, hiện dấu chấm than cảnh báo nếu gần đến giờ lấy món ăn</t>
+  </si>
+  <si>
+    <t>Thuật toán</t>
+  </si>
+  <si>
+    <t>Liên kết database và hiện thực thuật toán làm việc</t>
+  </si>
+  <si>
+    <t>Shop</t>
+  </si>
+  <si>
+    <t>Giống tìm kiếm ở Customer-&gt;Home</t>
+  </si>
+  <si>
+    <t>Thêm item</t>
+  </si>
+  <si>
+    <t>Thêm mới item lên database</t>
+  </si>
+  <si>
+    <t>Nhấn vào món ăn sẽ hiện ra dialog item_detail để chọn vào giỏ hàng -&gt; xác nhận cuối cùng</t>
+  </si>
+  <si>
+    <t>Chỉnh sửa hoặc xóa</t>
+  </si>
+  <si>
+    <t>Sửa item hoặc xóa item</t>
+  </si>
+  <si>
+    <t>Tìm kiếm theo MSSV</t>
+  </si>
+  <si>
+    <t>Khi nhập "30" thì chỉ hiển các MSSV có chứa "30"</t>
+  </si>
+  <si>
+    <t>Thêm coin</t>
+  </si>
+  <si>
+    <t>Nhấn vào SV muốn thêm coin, get dữ liệu money từ box trên (nhớ check null) và coin%10000==0</t>
+  </si>
+  <si>
+    <t>Profile</t>
+  </si>
+  <si>
+    <t>Xem lịch sử</t>
+  </si>
+  <si>
+    <t>Xem lại lịch sử nhân viên này đã nhận và làm các món ăn nào</t>
   </si>
 </sst>
 </file>
@@ -1011,7 +1159,7 @@
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1140,6 +1288,96 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="14" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="14" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="11" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="14" fontId="11" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="14" fontId="11" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="16" fontId="11" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="16" fontId="11" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -1149,104 +1387,17 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="14" fontId="11" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="14" fontId="11" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="14" fontId="11" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="16" fontId="11" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="16" fontId="11" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="14" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="14" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="16" fontId="11" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="16" fontId="11" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2400,7 +2551,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A3:I52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
@@ -2419,56 +2570,56 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:9" ht="25.8">
-      <c r="B3" s="91" t="s">
+      <c r="B3" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="91"/>
-      <c r="D3" s="91"/>
-      <c r="E3" s="91"/>
-      <c r="F3" s="91"/>
-      <c r="G3" s="91"/>
-      <c r="H3" s="91"/>
-      <c r="I3" s="91"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="72"/>
+      <c r="I3" s="72"/>
     </row>
     <row r="5" spans="1:9" ht="21">
-      <c r="B5" s="92" t="s">
+      <c r="B5" s="73" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="92"/>
-      <c r="D5" s="92"/>
-      <c r="E5" s="92"/>
-      <c r="F5" s="92"/>
-      <c r="G5" s="92"/>
-      <c r="H5" s="92"/>
-      <c r="I5" s="92"/>
+      <c r="C5" s="73"/>
+      <c r="D5" s="73"/>
+      <c r="E5" s="73"/>
+      <c r="F5" s="73"/>
+      <c r="G5" s="73"/>
+      <c r="H5" s="73"/>
+      <c r="I5" s="73"/>
     </row>
     <row r="7" spans="1:9" ht="18">
-      <c r="B7" s="96" t="s">
+      <c r="B7" s="77" t="s">
         <v>54</v>
       </c>
-      <c r="C7" s="98" t="s">
+      <c r="C7" s="82" t="s">
         <v>55</v>
       </c>
-      <c r="D7" s="100" t="s">
+      <c r="D7" s="87" t="s">
         <v>56</v>
       </c>
-      <c r="E7" s="102" t="s">
+      <c r="E7" s="89" t="s">
         <v>57</v>
       </c>
-      <c r="F7" s="93" t="s">
+      <c r="F7" s="74" t="s">
         <v>58</v>
       </c>
-      <c r="G7" s="94"/>
-      <c r="H7" s="95"/>
-      <c r="I7" s="104" t="s">
+      <c r="G7" s="75"/>
+      <c r="H7" s="76"/>
+      <c r="I7" s="91" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="18">
-      <c r="B8" s="97"/>
-      <c r="C8" s="99"/>
-      <c r="D8" s="101"/>
-      <c r="E8" s="103"/>
+      <c r="B8" s="78"/>
+      <c r="C8" s="83"/>
+      <c r="D8" s="88"/>
+      <c r="E8" s="90"/>
       <c r="F8" s="46" t="s">
         <v>60</v>
       </c>
@@ -2478,13 +2629,13 @@
       <c r="H8" s="47" t="s">
         <v>62</v>
       </c>
-      <c r="I8" s="105"/>
+      <c r="I8" s="92"/>
     </row>
     <row r="9" spans="1:9" ht="18">
-      <c r="B9" s="88" t="s">
+      <c r="B9" s="79" t="s">
         <v>90</v>
       </c>
-      <c r="C9" s="75" t="s">
+      <c r="C9" s="84" t="s">
         <v>94</v>
       </c>
       <c r="D9" s="48" t="s">
@@ -2503,8 +2654,8 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="18">
-      <c r="B10" s="89"/>
-      <c r="C10" s="76"/>
+      <c r="B10" s="80"/>
+      <c r="C10" s="85"/>
       <c r="D10" s="50" t="s">
         <v>65</v>
       </c>
@@ -2523,8 +2674,8 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="18">
-      <c r="B11" s="89"/>
-      <c r="C11" s="76"/>
+      <c r="B11" s="80"/>
+      <c r="C11" s="85"/>
       <c r="D11" s="50" t="s">
         <v>68</v>
       </c>
@@ -2541,8 +2692,8 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="18">
-      <c r="B12" s="89"/>
-      <c r="C12" s="76"/>
+      <c r="B12" s="80"/>
+      <c r="C12" s="85"/>
       <c r="D12" s="50" t="s">
         <v>70</v>
       </c>
@@ -2559,8 +2710,8 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="18.600000000000001" thickBot="1">
-      <c r="B13" s="90"/>
-      <c r="C13" s="77"/>
+      <c r="B13" s="81"/>
+      <c r="C13" s="86"/>
       <c r="D13" s="51" t="s">
         <v>71</v>
       </c>
@@ -2578,10 +2729,10 @@
     </row>
     <row r="14" spans="1:9" ht="18" customHeight="1">
       <c r="A14" s="52"/>
-      <c r="B14" s="79" t="s">
+      <c r="B14" s="93" t="s">
         <v>91</v>
       </c>
-      <c r="C14" s="72" t="s">
+      <c r="C14" s="102" t="s">
         <v>93</v>
       </c>
       <c r="D14" s="53" t="s">
@@ -2601,8 +2752,8 @@
     </row>
     <row r="15" spans="1:9" ht="18">
       <c r="A15" s="52"/>
-      <c r="B15" s="80"/>
-      <c r="C15" s="73"/>
+      <c r="B15" s="94"/>
+      <c r="C15" s="103"/>
       <c r="D15" s="55" t="s">
         <v>128</v>
       </c>
@@ -2620,8 +2771,8 @@
     </row>
     <row r="16" spans="1:9" ht="18">
       <c r="A16" s="52"/>
-      <c r="B16" s="80"/>
-      <c r="C16" s="73"/>
+      <c r="B16" s="94"/>
+      <c r="C16" s="103"/>
       <c r="D16" s="55" t="s">
         <v>131</v>
       </c>
@@ -2639,8 +2790,8 @@
     </row>
     <row r="17" spans="1:9" ht="18">
       <c r="A17" s="52"/>
-      <c r="B17" s="80"/>
-      <c r="C17" s="73"/>
+      <c r="B17" s="94"/>
+      <c r="C17" s="103"/>
       <c r="D17" s="55" t="s">
         <v>129</v>
       </c>
@@ -2658,8 +2809,8 @@
     </row>
     <row r="18" spans="1:9" ht="18.600000000000001" thickBot="1">
       <c r="A18" s="52"/>
-      <c r="B18" s="81"/>
-      <c r="C18" s="74"/>
+      <c r="B18" s="95"/>
+      <c r="C18" s="104"/>
       <c r="D18" s="56" t="s">
         <v>130</v>
       </c>
@@ -2677,10 +2828,10 @@
     </row>
     <row r="19" spans="1:9" ht="18.600000000000001" customHeight="1" thickBot="1">
       <c r="A19" s="52"/>
-      <c r="B19" s="82">
+      <c r="B19" s="96">
         <v>43712</v>
       </c>
-      <c r="C19" s="75" t="s">
+      <c r="C19" s="84" t="s">
         <v>92</v>
       </c>
       <c r="D19" s="48" t="s">
@@ -2700,8 +2851,8 @@
     </row>
     <row r="20" spans="1:9" ht="18.600000000000001" thickBot="1">
       <c r="A20" s="52"/>
-      <c r="B20" s="83"/>
-      <c r="C20" s="76"/>
+      <c r="B20" s="97"/>
+      <c r="C20" s="85"/>
       <c r="D20" s="50" t="s">
         <v>133</v>
       </c>
@@ -2719,8 +2870,8 @@
     </row>
     <row r="21" spans="1:9" ht="18.600000000000001" thickBot="1">
       <c r="A21" s="52"/>
-      <c r="B21" s="83"/>
-      <c r="C21" s="76"/>
+      <c r="B21" s="97"/>
+      <c r="C21" s="85"/>
       <c r="D21" s="50" t="s">
         <v>134</v>
       </c>
@@ -2738,8 +2889,8 @@
     </row>
     <row r="22" spans="1:9" ht="18.600000000000001" thickBot="1">
       <c r="A22" s="52"/>
-      <c r="B22" s="83"/>
-      <c r="C22" s="76"/>
+      <c r="B22" s="97"/>
+      <c r="C22" s="85"/>
       <c r="D22" s="50" t="s">
         <v>76</v>
       </c>
@@ -2757,8 +2908,8 @@
     </row>
     <row r="23" spans="1:9" ht="18.600000000000001" thickBot="1">
       <c r="A23" s="52"/>
-      <c r="B23" s="84"/>
-      <c r="C23" s="77"/>
+      <c r="B23" s="98"/>
+      <c r="C23" s="86"/>
       <c r="D23" s="51" t="s">
         <v>77</v>
       </c>
@@ -2776,10 +2927,10 @@
     </row>
     <row r="24" spans="1:9" ht="18">
       <c r="A24" s="52"/>
-      <c r="B24" s="85" t="s">
+      <c r="B24" s="99" t="s">
         <v>102</v>
       </c>
-      <c r="C24" s="72" t="s">
+      <c r="C24" s="102" t="s">
         <v>103</v>
       </c>
       <c r="D24" s="53" t="s">
@@ -2799,8 +2950,8 @@
     </row>
     <row r="25" spans="1:9" ht="18">
       <c r="A25" s="52"/>
-      <c r="B25" s="86"/>
-      <c r="C25" s="73"/>
+      <c r="B25" s="100"/>
+      <c r="C25" s="103"/>
       <c r="D25" s="55" t="s">
         <v>135</v>
       </c>
@@ -2818,8 +2969,8 @@
     </row>
     <row r="26" spans="1:9" ht="18">
       <c r="A26" s="52"/>
-      <c r="B26" s="86"/>
-      <c r="C26" s="73"/>
+      <c r="B26" s="100"/>
+      <c r="C26" s="103"/>
       <c r="D26" s="55" t="s">
         <v>136</v>
       </c>
@@ -2837,8 +2988,8 @@
     </row>
     <row r="27" spans="1:9" ht="18">
       <c r="A27" s="52"/>
-      <c r="B27" s="86"/>
-      <c r="C27" s="73"/>
+      <c r="B27" s="100"/>
+      <c r="C27" s="103"/>
       <c r="D27" s="55" t="s">
         <v>100</v>
       </c>
@@ -2856,8 +3007,8 @@
     </row>
     <row r="28" spans="1:9" ht="18">
       <c r="A28" s="52"/>
-      <c r="B28" s="87"/>
-      <c r="C28" s="78"/>
+      <c r="B28" s="101"/>
+      <c r="C28" s="105"/>
       <c r="D28" s="57" t="s">
         <v>101</v>
       </c>
@@ -2875,7 +3026,7 @@
     </row>
     <row r="29" spans="1:9" ht="18">
       <c r="A29" s="52"/>
-      <c r="B29" s="88" t="s">
+      <c r="B29" s="79" t="s">
         <v>125</v>
       </c>
       <c r="C29" s="106">
@@ -2898,8 +3049,8 @@
     </row>
     <row r="30" spans="1:9" ht="18">
       <c r="A30" s="52"/>
-      <c r="B30" s="89"/>
-      <c r="C30" s="76"/>
+      <c r="B30" s="80"/>
+      <c r="C30" s="85"/>
       <c r="D30" s="50" t="s">
         <v>138</v>
       </c>
@@ -2917,8 +3068,8 @@
     </row>
     <row r="31" spans="1:9" ht="18">
       <c r="A31" s="52"/>
-      <c r="B31" s="89"/>
-      <c r="C31" s="76"/>
+      <c r="B31" s="80"/>
+      <c r="C31" s="85"/>
       <c r="D31" s="50" t="s">
         <v>127</v>
       </c>
@@ -2936,8 +3087,8 @@
     </row>
     <row r="32" spans="1:9" ht="18">
       <c r="A32" s="52"/>
-      <c r="B32" s="89"/>
-      <c r="C32" s="76"/>
+      <c r="B32" s="80"/>
+      <c r="C32" s="85"/>
       <c r="D32" s="50" t="s">
         <v>140</v>
       </c>
@@ -2955,8 +3106,8 @@
     </row>
     <row r="33" spans="1:9" ht="18">
       <c r="A33" s="52"/>
-      <c r="B33" s="90"/>
-      <c r="C33" s="77"/>
+      <c r="B33" s="81"/>
+      <c r="C33" s="86"/>
       <c r="D33" s="51" t="s">
         <v>137</v>
       </c>
@@ -2974,7 +3125,7 @@
     </row>
     <row r="34" spans="1:9" ht="18">
       <c r="A34" s="52"/>
-      <c r="B34" s="85">
+      <c r="B34" s="99">
         <v>43588</v>
       </c>
       <c r="C34" s="107">
@@ -2997,8 +3148,8 @@
     </row>
     <row r="35" spans="1:9" ht="18">
       <c r="A35" s="52"/>
-      <c r="B35" s="86"/>
-      <c r="C35" s="73"/>
+      <c r="B35" s="100"/>
+      <c r="C35" s="103"/>
       <c r="D35" s="55" t="s">
         <v>143</v>
       </c>
@@ -3016,8 +3167,8 @@
     </row>
     <row r="36" spans="1:9" ht="18">
       <c r="A36" s="52"/>
-      <c r="B36" s="86"/>
-      <c r="C36" s="73"/>
+      <c r="B36" s="100"/>
+      <c r="C36" s="103"/>
       <c r="D36" s="55" t="s">
         <v>139</v>
       </c>
@@ -3035,8 +3186,8 @@
     </row>
     <row r="37" spans="1:9" ht="18">
       <c r="A37" s="52"/>
-      <c r="B37" s="86"/>
-      <c r="C37" s="73"/>
+      <c r="B37" s="100"/>
+      <c r="C37" s="103"/>
       <c r="D37" s="55" t="s">
         <v>142</v>
       </c>
@@ -3054,8 +3205,8 @@
     </row>
     <row r="38" spans="1:9" ht="18.600000000000001" thickBot="1">
       <c r="A38" s="52"/>
-      <c r="B38" s="87"/>
-      <c r="C38" s="78"/>
+      <c r="B38" s="101"/>
+      <c r="C38" s="105"/>
       <c r="D38" s="57" t="s">
         <v>141</v>
       </c>
@@ -3221,6 +3372,16 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="C14:C18"/>
+    <mergeCell ref="C19:C23"/>
+    <mergeCell ref="C24:C28"/>
+    <mergeCell ref="C29:C33"/>
+    <mergeCell ref="C34:C38"/>
+    <mergeCell ref="B14:B18"/>
+    <mergeCell ref="B19:B23"/>
+    <mergeCell ref="B24:B28"/>
+    <mergeCell ref="B29:B33"/>
+    <mergeCell ref="B34:B38"/>
     <mergeCell ref="B3:I3"/>
     <mergeCell ref="B5:I5"/>
     <mergeCell ref="F7:H7"/>
@@ -3231,18 +3392,458 @@
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="E7:E8"/>
     <mergeCell ref="I7:I8"/>
-    <mergeCell ref="B14:B18"/>
-    <mergeCell ref="B19:B23"/>
-    <mergeCell ref="B24:B28"/>
-    <mergeCell ref="B29:B33"/>
-    <mergeCell ref="B34:B38"/>
-    <mergeCell ref="C14:C18"/>
-    <mergeCell ref="C19:C23"/>
-    <mergeCell ref="C24:C28"/>
-    <mergeCell ref="C29:C33"/>
-    <mergeCell ref="C34:C38"/>
   </mergeCells>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37AA2E22-B916-4D99-A156-90D9CC0DC7BC}">
+  <dimension ref="B2:H28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="80.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8" ht="18">
+      <c r="B2" s="108" t="s">
+        <v>149</v>
+      </c>
+      <c r="C2" s="108" t="s">
+        <v>150</v>
+      </c>
+      <c r="D2" s="108" t="s">
+        <v>145</v>
+      </c>
+      <c r="E2" s="108" t="s">
+        <v>155</v>
+      </c>
+      <c r="F2" s="108" t="s">
+        <v>146</v>
+      </c>
+      <c r="G2" s="108" t="s">
+        <v>147</v>
+      </c>
+      <c r="H2" s="108" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8">
+      <c r="B3" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8">
+      <c r="B4" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8">
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8">
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="H6" s="15" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8">
+      <c r="B7" s="15"/>
+      <c r="C7" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="H7" s="15" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8">
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8">
+      <c r="B9" s="15"/>
+      <c r="C9" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="H9" s="15" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8">
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="H10" s="15" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8">
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15" t="s">
+        <v>176</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="H11" s="15" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8">
+      <c r="B12" s="15"/>
+      <c r="C12" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="H12" s="15" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8">
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="H13" s="15" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8">
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="H14" s="15" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8">
+      <c r="B15" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>178</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="H15" s="15" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8">
+      <c r="B16" s="15"/>
+      <c r="C16" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="H16" s="15" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8">
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="H17" s="15" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8">
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="H18" s="15" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8">
+      <c r="B19" s="15"/>
+      <c r="C19" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="H19" s="15" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8">
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="H20" s="15" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8">
+      <c r="B21" s="15"/>
+      <c r="C21" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="H21" s="15" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8">
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+    </row>
+    <row r="23" spans="2:8">
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+    </row>
+    <row r="24" spans="2:8">
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
+    </row>
+    <row r="25" spans="2:8">
+      <c r="B25" s="15"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="15"/>
+    </row>
+    <row r="26" spans="2:8">
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="15"/>
+    </row>
+    <row r="27" spans="2:8">
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
+    </row>
+    <row r="28" spans="2:8">
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Thêm tính năng order
</commit_message>
<xml_diff>
--- a/N65_HappyLunch.xlsx
+++ b/N65_HappyLunch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\apk\git\Happy_Lunch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D87E537-0B5B-4903-AC78-B751BCBC2E18}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA966A40-A1E0-40A0-8E95-472AF7AA5AFF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Profile" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="285">
   <si>
     <t>NHÓM 65: HAPPY LUNCH</t>
   </si>
@@ -471,9 +471,6 @@
     <t>Tình trạng</t>
   </si>
   <si>
-    <t>Chưa hiện thực</t>
-  </si>
-  <si>
     <t>Loại</t>
   </si>
   <si>
@@ -540,9 +537,6 @@
     <t>Git</t>
   </si>
   <si>
-    <t>Chưa đồng bộ</t>
-  </si>
-  <si>
     <t>Login</t>
   </si>
   <si>
@@ -868,6 +862,24 @@
   </si>
   <si>
     <t>Một số chức năng (cụ thể ở Sheet4)</t>
+  </si>
+  <si>
+    <t>Đã đồng bộ</t>
+  </si>
+  <si>
+    <t>Hoàn thành</t>
+  </si>
+  <si>
+    <t>Bỏ</t>
+  </si>
+  <si>
+    <t>Chưa</t>
+  </si>
+  <si>
+    <t>Gần xong</t>
+  </si>
+  <si>
+    <t>Chưa fix bug</t>
   </si>
 </sst>
 </file>
@@ -2307,7 +2319,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B3:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
@@ -3648,7 +3660,7 @@
         <v>43599</v>
       </c>
       <c r="D39" s="74" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="E39" s="48" t="s">
         <v>9</v>
@@ -3663,7 +3675,7 @@
       <c r="B40" s="82"/>
       <c r="C40" s="85"/>
       <c r="D40" s="74" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="E40" s="50" t="s">
         <v>14</v>
@@ -3678,7 +3690,7 @@
       <c r="B41" s="82"/>
       <c r="C41" s="85"/>
       <c r="D41" s="74" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="E41" s="50" t="s">
         <v>19</v>
@@ -3693,7 +3705,7 @@
       <c r="B42" s="82"/>
       <c r="C42" s="85"/>
       <c r="D42" s="74" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="E42" s="50" t="s">
         <v>24</v>
@@ -3708,7 +3720,7 @@
       <c r="B43" s="83"/>
       <c r="C43" s="86"/>
       <c r="D43" s="74" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="E43" s="51" t="s">
         <v>29</v>
@@ -3845,8 +3857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37AA2E22-B916-4D99-A156-90D9CC0DC7BC}">
   <dimension ref="B2:H28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3854,7 +3866,7 @@
     <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="77.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="80.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.44140625" bestFit="1" customWidth="1"/>
@@ -3862,16 +3874,16 @@
   <sheetData>
     <row r="2" spans="2:8" ht="36">
       <c r="B2" s="66" t="s">
+        <v>148</v>
+      </c>
+      <c r="C2" s="66" t="s">
         <v>149</v>
-      </c>
-      <c r="C2" s="66" t="s">
-        <v>150</v>
       </c>
       <c r="D2" s="66" t="s">
         <v>145</v>
       </c>
       <c r="E2" s="66" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F2" s="66" t="s">
         <v>146</v>
@@ -3880,385 +3892,363 @@
         <v>147</v>
       </c>
       <c r="H2" s="66" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" spans="2:8">
       <c r="B3" s="67" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C3" s="67" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D3" s="67" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E3" s="67"/>
       <c r="F3" s="67" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G3" s="67" t="s">
-        <v>148</v>
+        <v>280</v>
       </c>
       <c r="H3" s="67" t="s">
-        <v>171</v>
+        <v>279</v>
       </c>
     </row>
     <row r="4" spans="2:8">
       <c r="B4" s="67" t="s">
+        <v>150</v>
+      </c>
+      <c r="C4" s="67" t="s">
         <v>151</v>
       </c>
-      <c r="C4" s="67" t="s">
+      <c r="D4" s="67" t="s">
         <v>152</v>
-      </c>
-      <c r="D4" s="67" t="s">
-        <v>153</v>
       </c>
       <c r="E4" s="67"/>
       <c r="F4" s="67" t="s">
-        <v>191</v>
-      </c>
-      <c r="G4" s="67" t="s">
-        <v>148</v>
-      </c>
-      <c r="H4" s="67" t="s">
-        <v>171</v>
-      </c>
+        <v>189</v>
+      </c>
+      <c r="G4" s="67"/>
+      <c r="H4" s="67"/>
     </row>
     <row r="5" spans="2:8">
       <c r="B5" s="67"/>
       <c r="C5" s="67"/>
       <c r="D5" s="67" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E5" s="67"/>
       <c r="F5" s="67" t="s">
-        <v>191</v>
-      </c>
-      <c r="G5" s="67" t="s">
-        <v>148</v>
-      </c>
-      <c r="H5" s="67" t="s">
-        <v>171</v>
-      </c>
+        <v>189</v>
+      </c>
+      <c r="G5" s="67"/>
+      <c r="H5" s="67"/>
     </row>
     <row r="6" spans="2:8">
       <c r="B6" s="67"/>
       <c r="C6" s="67"/>
       <c r="D6" s="67" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E6" s="67" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F6" s="67" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="G6" s="67" t="s">
-        <v>148</v>
+        <v>280</v>
       </c>
       <c r="H6" s="67" t="s">
-        <v>171</v>
+        <v>279</v>
       </c>
     </row>
     <row r="7" spans="2:8">
       <c r="B7" s="67"/>
       <c r="C7" s="67" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D7" s="67" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E7" s="67" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F7" s="67" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="G7" s="67" t="s">
-        <v>148</v>
+        <v>280</v>
       </c>
       <c r="H7" s="67" t="s">
-        <v>171</v>
+        <v>279</v>
       </c>
     </row>
     <row r="8" spans="2:8">
       <c r="B8" s="67"/>
       <c r="C8" s="67"/>
       <c r="D8" s="67" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E8" s="67" t="s">
-        <v>162</v>
-      </c>
-      <c r="F8" s="67"/>
+        <v>161</v>
+      </c>
+      <c r="F8" s="67" t="s">
+        <v>190</v>
+      </c>
       <c r="G8" s="67" t="s">
-        <v>148</v>
+        <v>280</v>
       </c>
       <c r="H8" s="67" t="s">
-        <v>171</v>
+        <v>279</v>
       </c>
     </row>
     <row r="9" spans="2:8">
       <c r="B9" s="67"/>
       <c r="C9" s="67" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D9" s="67" t="s">
+        <v>159</v>
+      </c>
+      <c r="E9" s="67" t="s">
         <v>160</v>
       </c>
-      <c r="E9" s="67" t="s">
-        <v>161</v>
-      </c>
-      <c r="F9" s="67"/>
+      <c r="F9" s="67" t="s">
+        <v>190</v>
+      </c>
       <c r="G9" s="67" t="s">
-        <v>148</v>
+        <v>280</v>
       </c>
       <c r="H9" s="67" t="s">
-        <v>171</v>
+        <v>279</v>
       </c>
     </row>
     <row r="10" spans="2:8">
       <c r="B10" s="67"/>
       <c r="C10" s="67"/>
       <c r="D10" s="67" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E10" s="67" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F10" s="67" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="G10" s="67" t="s">
-        <v>148</v>
+        <v>280</v>
       </c>
       <c r="H10" s="67" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" ht="28.8">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8">
       <c r="B11" s="67"/>
       <c r="C11" s="67"/>
       <c r="D11" s="67" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E11" s="67" t="s">
-        <v>177</v>
-      </c>
-      <c r="F11" s="67" t="s">
-        <v>193</v>
-      </c>
+        <v>175</v>
+      </c>
+      <c r="F11" s="67"/>
       <c r="G11" s="67" t="s">
-        <v>148</v>
+        <v>281</v>
       </c>
       <c r="H11" s="67" t="s">
-        <v>171</v>
+        <v>279</v>
       </c>
     </row>
     <row r="12" spans="2:8">
       <c r="B12" s="67"/>
       <c r="C12" s="67" t="s">
+        <v>163</v>
+      </c>
+      <c r="D12" s="67" t="s">
         <v>164</v>
       </c>
-      <c r="D12" s="67" t="s">
+      <c r="E12" s="67" t="s">
         <v>165</v>
       </c>
-      <c r="E12" s="67" t="s">
-        <v>166</v>
-      </c>
       <c r="F12" s="67" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="G12" s="67" t="s">
-        <v>148</v>
+        <v>280</v>
       </c>
       <c r="H12" s="67" t="s">
-        <v>171</v>
+        <v>282</v>
       </c>
     </row>
     <row r="13" spans="2:8">
       <c r="B13" s="67"/>
       <c r="C13" s="67"/>
       <c r="D13" s="67" t="s">
+        <v>166</v>
+      </c>
+      <c r="E13" s="67" t="s">
         <v>167</v>
       </c>
-      <c r="E13" s="67" t="s">
-        <v>168</v>
-      </c>
       <c r="F13" s="67" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="G13" s="67" t="s">
-        <v>148</v>
+        <v>280</v>
       </c>
       <c r="H13" s="67" t="s">
-        <v>171</v>
+        <v>282</v>
       </c>
     </row>
     <row r="14" spans="2:8">
       <c r="B14" s="67"/>
       <c r="C14" s="67"/>
       <c r="D14" s="67" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E14" s="67" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F14" s="67" t="s">
-        <v>196</v>
-      </c>
-      <c r="G14" s="67" t="s">
-        <v>148</v>
-      </c>
-      <c r="H14" s="67" t="s">
-        <v>171</v>
-      </c>
+        <v>194</v>
+      </c>
+      <c r="G14" s="67"/>
+      <c r="H14" s="67"/>
     </row>
     <row r="15" spans="2:8">
       <c r="B15" s="67" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C15" s="67" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D15" s="67" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E15" s="67" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F15" s="67" t="s">
-        <v>193</v>
-      </c>
-      <c r="G15" s="67" t="s">
-        <v>148</v>
-      </c>
-      <c r="H15" s="67" t="s">
-        <v>171</v>
-      </c>
+        <v>191</v>
+      </c>
+      <c r="G15" s="67"/>
+      <c r="H15" s="67"/>
     </row>
     <row r="16" spans="2:8">
       <c r="B16" s="67"/>
       <c r="C16" s="67" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D16" s="67" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E16" s="67" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F16" s="67" t="s">
-        <v>191</v>
-      </c>
-      <c r="G16" s="67" t="s">
-        <v>148</v>
-      </c>
-      <c r="H16" s="67" t="s">
-        <v>171</v>
-      </c>
+        <v>189</v>
+      </c>
+      <c r="G16" s="67"/>
+      <c r="H16" s="67"/>
     </row>
     <row r="17" spans="2:8">
       <c r="B17" s="67"/>
       <c r="C17" s="67"/>
       <c r="D17" s="67" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E17" s="67" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F17" s="67" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G17" s="67" t="s">
-        <v>148</v>
+        <v>280</v>
       </c>
       <c r="H17" s="67" t="s">
-        <v>171</v>
+        <v>282</v>
       </c>
     </row>
     <row r="18" spans="2:8">
       <c r="B18" s="67"/>
       <c r="C18" s="67"/>
       <c r="D18" s="67" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E18" s="67" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F18" s="67" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G18" s="67" t="s">
-        <v>148</v>
+        <v>283</v>
       </c>
       <c r="H18" s="67" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" ht="28.8">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" ht="15" customHeight="1">
       <c r="B19" s="67"/>
       <c r="C19" s="67" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D19" s="67" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E19" s="67" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F19" s="67" t="s">
-        <v>197</v>
-      </c>
-      <c r="G19" s="67" t="s">
-        <v>148</v>
-      </c>
-      <c r="H19" s="67" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" ht="28.8">
+        <v>195</v>
+      </c>
+      <c r="G19" s="67"/>
+      <c r="H19" s="67"/>
+    </row>
+    <row r="20" spans="2:8">
       <c r="B20" s="67"/>
       <c r="C20" s="67"/>
       <c r="D20" s="67" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E20" s="67" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F20" s="68" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="G20" s="67" t="s">
-        <v>148</v>
+        <v>284</v>
       </c>
       <c r="H20" s="67" t="s">
-        <v>171</v>
+        <v>279</v>
       </c>
     </row>
     <row r="21" spans="2:8">
       <c r="B21" s="67" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C21" s="67"/>
       <c r="D21" s="67"/>
       <c r="E21" s="67"/>
       <c r="F21" s="67" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="G21" s="67"/>
       <c r="H21" s="67"/>
     </row>
     <row r="22" spans="2:8">
       <c r="B22" s="69" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C22" s="15"/>
       <c r="D22" s="15"/>
       <c r="E22" s="15"/>
       <c r="F22" s="69" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="G22" s="15"/>
       <c r="H22" s="15"/>
@@ -4345,7 +4335,7 @@
   <sheetData>
     <row r="1" spans="2:10" ht="28.8">
       <c r="B1" s="118" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C1" s="118"/>
       <c r="D1" s="118"/>
@@ -4361,28 +4351,28 @@
         <v>2</v>
       </c>
       <c r="C3" s="71" t="s">
+        <v>199</v>
+      </c>
+      <c r="D3" s="71" t="s">
+        <v>200</v>
+      </c>
+      <c r="E3" s="71" t="s">
         <v>201</v>
       </c>
-      <c r="D3" s="71" t="s">
+      <c r="F3" s="71" t="s">
         <v>202</v>
       </c>
-      <c r="E3" s="71" t="s">
+      <c r="G3" s="71" t="s">
         <v>203</v>
       </c>
-      <c r="F3" s="71" t="s">
+      <c r="H3" s="71" t="s">
         <v>204</v>
       </c>
-      <c r="G3" s="71" t="s">
+      <c r="I3" s="72" t="s">
         <v>205</v>
       </c>
-      <c r="H3" s="71" t="s">
+      <c r="J3" s="71" t="s">
         <v>206</v>
-      </c>
-      <c r="I3" s="72" t="s">
-        <v>207</v>
-      </c>
-      <c r="J3" s="71" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="4" spans="2:10" ht="28.8">
@@ -4390,16 +4380,16 @@
         <v>1</v>
       </c>
       <c r="C4" s="73" t="s">
+        <v>207</v>
+      </c>
+      <c r="D4" s="73" t="s">
+        <v>208</v>
+      </c>
+      <c r="E4" s="73" t="s">
         <v>209</v>
       </c>
-      <c r="D4" s="73" t="s">
+      <c r="F4" s="73" t="s">
         <v>210</v>
-      </c>
-      <c r="E4" s="73" t="s">
-        <v>211</v>
-      </c>
-      <c r="F4" s="73" t="s">
-        <v>212</v>
       </c>
       <c r="G4" s="73" t="s">
         <v>44</v>
@@ -4411,7 +4401,7 @@
         <v>65</v>
       </c>
       <c r="J4" s="73" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="5" spans="2:10" ht="28.8">
@@ -4419,16 +4409,16 @@
         <v>2</v>
       </c>
       <c r="C5" s="73" t="s">
+        <v>212</v>
+      </c>
+      <c r="D5" s="73" t="s">
+        <v>213</v>
+      </c>
+      <c r="E5" s="73" t="s">
         <v>214</v>
       </c>
-      <c r="D5" s="73" t="s">
-        <v>215</v>
-      </c>
-      <c r="E5" s="73" t="s">
-        <v>216</v>
-      </c>
       <c r="F5" s="73" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G5" s="73" t="s">
         <v>44</v>
@@ -4440,7 +4430,7 @@
         <v>65</v>
       </c>
       <c r="J5" s="73" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="28.8">
@@ -4448,16 +4438,16 @@
         <v>3</v>
       </c>
       <c r="C6" s="73" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D6" s="73" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E6" s="73" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F6" s="73" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G6" s="73" t="s">
         <v>44</v>
@@ -4469,7 +4459,7 @@
         <v>65</v>
       </c>
       <c r="J6" s="73" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="7" spans="2:10" ht="28.8">
@@ -4477,16 +4467,16 @@
         <v>4</v>
       </c>
       <c r="C7" s="73" t="s">
+        <v>217</v>
+      </c>
+      <c r="D7" s="73" t="s">
+        <v>218</v>
+      </c>
+      <c r="E7" s="73" t="s">
         <v>219</v>
       </c>
-      <c r="D7" s="73" t="s">
-        <v>220</v>
-      </c>
-      <c r="E7" s="73" t="s">
-        <v>221</v>
-      </c>
       <c r="F7" s="73" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G7" s="73" t="s">
         <v>44</v>
@@ -4498,13 +4488,13 @@
         <v>65</v>
       </c>
       <c r="J7" s="73" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="8" spans="2:10">
       <c r="B8" s="70"/>
       <c r="C8" s="119" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D8" s="120"/>
       <c r="E8" s="121"/>
@@ -4519,28 +4509,28 @@
         <v>5</v>
       </c>
       <c r="C9" s="73" t="s">
+        <v>221</v>
+      </c>
+      <c r="D9" s="73" t="s">
+        <v>222</v>
+      </c>
+      <c r="E9" s="73" t="s">
         <v>223</v>
       </c>
-      <c r="D9" s="73" t="s">
+      <c r="F9" s="73" t="s">
         <v>224</v>
       </c>
-      <c r="E9" s="73" t="s">
+      <c r="G9" s="73" t="s">
         <v>225</v>
       </c>
-      <c r="F9" s="73" t="s">
+      <c r="H9" s="73" t="s">
         <v>226</v>
-      </c>
-      <c r="G9" s="73" t="s">
-        <v>227</v>
-      </c>
-      <c r="H9" s="73" t="s">
-        <v>228</v>
       </c>
       <c r="I9" s="73">
         <v>65</v>
       </c>
       <c r="J9" s="73" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="10" spans="2:10" ht="57.6">
@@ -4548,26 +4538,26 @@
         <v>6</v>
       </c>
       <c r="C10" s="73" t="s">
+        <v>228</v>
+      </c>
+      <c r="D10" s="73" t="s">
+        <v>229</v>
+      </c>
+      <c r="E10" s="73" t="s">
         <v>230</v>
       </c>
-      <c r="D10" s="73" t="s">
+      <c r="F10" s="73" t="s">
         <v>231</v>
       </c>
-      <c r="E10" s="73" t="s">
+      <c r="G10" s="73" t="s">
         <v>232</v>
-      </c>
-      <c r="F10" s="73" t="s">
-        <v>233</v>
-      </c>
-      <c r="G10" s="73" t="s">
-        <v>234</v>
       </c>
       <c r="H10" s="73"/>
       <c r="I10" s="73">
         <v>65</v>
       </c>
       <c r="J10" s="73" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="100.8">
@@ -4575,28 +4565,28 @@
         <v>7</v>
       </c>
       <c r="C11" s="73" t="s">
+        <v>234</v>
+      </c>
+      <c r="D11" s="73" t="s">
+        <v>235</v>
+      </c>
+      <c r="E11" s="73" t="s">
         <v>236</v>
       </c>
-      <c r="D11" s="73" t="s">
+      <c r="F11" s="73" t="s">
+        <v>224</v>
+      </c>
+      <c r="G11" s="73" t="s">
         <v>237</v>
       </c>
-      <c r="E11" s="73" t="s">
+      <c r="H11" s="73" t="s">
         <v>238</v>
-      </c>
-      <c r="F11" s="73" t="s">
-        <v>226</v>
-      </c>
-      <c r="G11" s="73" t="s">
-        <v>239</v>
-      </c>
-      <c r="H11" s="73" t="s">
-        <v>240</v>
       </c>
       <c r="I11" s="73">
         <v>65</v>
       </c>
       <c r="J11" s="73" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="12" spans="2:10" ht="57.6">
@@ -4604,28 +4594,28 @@
         <v>8</v>
       </c>
       <c r="C12" s="73" t="s">
+        <v>240</v>
+      </c>
+      <c r="D12" s="73" t="s">
+        <v>241</v>
+      </c>
+      <c r="E12" s="73" t="s">
         <v>242</v>
       </c>
-      <c r="D12" s="73" t="s">
+      <c r="F12" s="73" t="s">
+        <v>224</v>
+      </c>
+      <c r="G12" s="73" t="s">
         <v>243</v>
       </c>
-      <c r="E12" s="73" t="s">
+      <c r="H12" s="73" t="s">
         <v>244</v>
-      </c>
-      <c r="F12" s="73" t="s">
-        <v>226</v>
-      </c>
-      <c r="G12" s="73" t="s">
-        <v>245</v>
-      </c>
-      <c r="H12" s="73" t="s">
-        <v>246</v>
       </c>
       <c r="I12" s="73">
         <v>65</v>
       </c>
       <c r="J12" s="73" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="13" spans="2:10" ht="28.8">
@@ -4633,16 +4623,16 @@
         <v>9</v>
       </c>
       <c r="C13" s="73" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D13" s="73" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E13" s="73" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="F13" s="73" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G13" s="73" t="s">
         <v>44</v>
@@ -4654,7 +4644,7 @@
         <v>65</v>
       </c>
       <c r="J13" s="73" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="14" spans="2:10" ht="28.8">
@@ -4662,16 +4652,16 @@
         <v>10</v>
       </c>
       <c r="C14" s="73" t="s">
+        <v>248</v>
+      </c>
+      <c r="D14" s="73" t="s">
+        <v>249</v>
+      </c>
+      <c r="E14" s="73" t="s">
         <v>250</v>
       </c>
-      <c r="D14" s="73" t="s">
-        <v>251</v>
-      </c>
-      <c r="E14" s="73" t="s">
-        <v>252</v>
-      </c>
       <c r="F14" s="73" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G14" s="73" t="s">
         <v>44</v>
@@ -4683,7 +4673,7 @@
         <v>65</v>
       </c>
       <c r="J14" s="73" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="15" spans="2:10" ht="43.2">
@@ -4691,16 +4681,16 @@
         <v>11</v>
       </c>
       <c r="C15" s="73" t="s">
+        <v>251</v>
+      </c>
+      <c r="D15" s="73" t="s">
+        <v>252</v>
+      </c>
+      <c r="E15" s="73" t="s">
         <v>253</v>
       </c>
-      <c r="D15" s="73" t="s">
-        <v>254</v>
-      </c>
-      <c r="E15" s="73" t="s">
-        <v>255</v>
-      </c>
       <c r="F15" s="73" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G15" s="73" t="s">
         <v>44</v>
@@ -4712,7 +4702,7 @@
         <v>65</v>
       </c>
       <c r="J15" s="73" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="16" spans="2:10" ht="28.8">
@@ -4720,28 +4710,28 @@
         <v>12</v>
       </c>
       <c r="C16" s="73" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D16" s="73" t="s">
+        <v>254</v>
+      </c>
+      <c r="E16" s="73" t="s">
+        <v>255</v>
+      </c>
+      <c r="F16" s="73" t="s">
+        <v>224</v>
+      </c>
+      <c r="G16" s="73" t="s">
         <v>256</v>
       </c>
-      <c r="E16" s="73" t="s">
+      <c r="H16" s="73" t="s">
         <v>257</v>
-      </c>
-      <c r="F16" s="73" t="s">
-        <v>226</v>
-      </c>
-      <c r="G16" s="73" t="s">
-        <v>258</v>
-      </c>
-      <c r="H16" s="73" t="s">
-        <v>259</v>
       </c>
       <c r="I16" s="73">
         <v>65</v>
       </c>
       <c r="J16" s="73" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="17" spans="2:10" ht="43.2">
@@ -4749,16 +4739,16 @@
         <v>13</v>
       </c>
       <c r="C17" s="73" t="s">
+        <v>258</v>
+      </c>
+      <c r="D17" s="73" t="s">
+        <v>259</v>
+      </c>
+      <c r="E17" s="73" t="s">
         <v>260</v>
       </c>
-      <c r="D17" s="73" t="s">
-        <v>261</v>
-      </c>
-      <c r="E17" s="73" t="s">
-        <v>262</v>
-      </c>
       <c r="F17" s="73" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G17" s="73" t="s">
         <v>44</v>
@@ -4770,13 +4760,13 @@
         <v>65</v>
       </c>
       <c r="J17" s="73" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="18" spans="2:10">
       <c r="B18" s="70"/>
       <c r="C18" s="119" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D18" s="120"/>
       <c r="E18" s="121"/>
@@ -4791,16 +4781,16 @@
         <v>14</v>
       </c>
       <c r="C19" s="73" t="s">
+        <v>262</v>
+      </c>
+      <c r="D19" s="73" t="s">
+        <v>263</v>
+      </c>
+      <c r="E19" s="73" t="s">
         <v>264</v>
       </c>
-      <c r="D19" s="73" t="s">
-        <v>265</v>
-      </c>
-      <c r="E19" s="73" t="s">
-        <v>266</v>
-      </c>
       <c r="F19" s="73" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G19" s="73" t="s">
         <v>44</v>
@@ -4812,7 +4802,7 @@
         <v>65</v>
       </c>
       <c r="J19" s="73" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="20" spans="2:10" ht="57.6">
@@ -4820,16 +4810,16 @@
         <v>15</v>
       </c>
       <c r="C20" s="73" t="s">
+        <v>265</v>
+      </c>
+      <c r="D20" s="73" t="s">
+        <v>266</v>
+      </c>
+      <c r="E20" s="73" t="s">
         <v>267</v>
       </c>
-      <c r="D20" s="73" t="s">
-        <v>268</v>
-      </c>
-      <c r="E20" s="73" t="s">
-        <v>269</v>
-      </c>
       <c r="F20" s="73" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G20" s="73" t="s">
         <v>44</v>
@@ -4841,7 +4831,7 @@
         <v>65</v>
       </c>
       <c r="J20" s="73" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="21" spans="2:10" ht="57.6">
@@ -4849,28 +4839,28 @@
         <v>16</v>
       </c>
       <c r="C21" s="73" t="s">
+        <v>221</v>
+      </c>
+      <c r="D21" s="73" t="s">
+        <v>222</v>
+      </c>
+      <c r="E21" s="73" t="s">
         <v>223</v>
       </c>
-      <c r="D21" s="73" t="s">
+      <c r="F21" s="73" t="s">
         <v>224</v>
       </c>
-      <c r="E21" s="73" t="s">
+      <c r="G21" s="73" t="s">
         <v>225</v>
       </c>
-      <c r="F21" s="73" t="s">
+      <c r="H21" s="73" t="s">
         <v>226</v>
-      </c>
-      <c r="G21" s="73" t="s">
-        <v>227</v>
-      </c>
-      <c r="H21" s="73" t="s">
-        <v>228</v>
       </c>
       <c r="I21" s="73">
         <v>65</v>
       </c>
       <c r="J21" s="73" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="22" spans="2:10" ht="28.8">
@@ -4878,16 +4868,16 @@
         <v>17</v>
       </c>
       <c r="C22" s="73" t="s">
+        <v>268</v>
+      </c>
+      <c r="D22" s="73" t="s">
+        <v>269</v>
+      </c>
+      <c r="E22" s="73" t="s">
         <v>270</v>
       </c>
-      <c r="D22" s="73" t="s">
-        <v>271</v>
-      </c>
-      <c r="E22" s="73" t="s">
-        <v>272</v>
-      </c>
       <c r="F22" s="73" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G22" s="73" t="s">
         <v>44</v>
@@ -4899,7 +4889,7 @@
         <v>65</v>
       </c>
       <c r="J22" s="73" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="23" spans="2:10" ht="43.2">
@@ -4907,28 +4897,28 @@
         <v>18</v>
       </c>
       <c r="C23" s="73" t="s">
+        <v>271</v>
+      </c>
+      <c r="D23" s="73" t="s">
+        <v>272</v>
+      </c>
+      <c r="E23" s="73" t="s">
+        <v>214</v>
+      </c>
+      <c r="F23" s="73" t="s">
+        <v>224</v>
+      </c>
+      <c r="G23" s="73" t="s">
         <v>273</v>
       </c>
-      <c r="D23" s="73" t="s">
+      <c r="H23" s="73" t="s">
         <v>274</v>
-      </c>
-      <c r="E23" s="73" t="s">
-        <v>216</v>
-      </c>
-      <c r="F23" s="73" t="s">
-        <v>226</v>
-      </c>
-      <c r="G23" s="73" t="s">
-        <v>275</v>
-      </c>
-      <c r="H23" s="73" t="s">
-        <v>276</v>
       </c>
       <c r="I23" s="73">
         <v>65</v>
       </c>
       <c r="J23" s="73" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="24" spans="2:10" ht="28.8">
@@ -4936,16 +4926,16 @@
         <v>19</v>
       </c>
       <c r="C24" s="73" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D24" s="73" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E24" s="73" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="F24" s="73" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G24" s="73" t="s">
         <v>44</v>
@@ -4957,7 +4947,7 @@
         <v>65</v>
       </c>
       <c r="J24" s="73" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="25" spans="2:10" ht="43.2">
@@ -4965,16 +4955,16 @@
         <v>20</v>
       </c>
       <c r="C25" s="73" t="s">
+        <v>258</v>
+      </c>
+      <c r="D25" s="73" t="s">
+        <v>277</v>
+      </c>
+      <c r="E25" s="73" t="s">
         <v>260</v>
       </c>
-      <c r="D25" s="73" t="s">
-        <v>279</v>
-      </c>
-      <c r="E25" s="73" t="s">
-        <v>262</v>
-      </c>
       <c r="F25" s="73" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G25" s="73" t="s">
         <v>44</v>
@@ -4986,7 +4976,7 @@
         <v>65</v>
       </c>
       <c r="J25" s="73" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>

</xml_diff>